<commit_message>
starting operational Iridium9603NBeacon_V5M arduiono code
</commit_message>
<xml_diff>
--- a/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
+++ b/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prl242\repositories\Iridium_9603_Beacon\Eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A460677-7658-411C-BA1F-6A202EAB6D8D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93B384A-365D-4006-B323-CC24BED97B06}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{3D564F82-D3D8-4CC0-A9F4-2EE497ABD49A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="255">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -771,9 +771,6 @@
     <t>J610-ND</t>
   </si>
   <si>
-    <t>Bulkhead Version</t>
-  </si>
-  <si>
     <t>4POS 2.5MM</t>
   </si>
   <si>
@@ -853,6 +850,30 @@
   </si>
   <si>
     <t>500R14N120JV4T</t>
+  </si>
+  <si>
+    <t>LCS_032_CTP</t>
+  </si>
+  <si>
+    <t>LIGHTPIPE THREADED</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>LCS_032_CTP-ND</t>
+  </si>
+  <si>
+    <t>Bulkhead Version, Enclosure Cutout: 7 mm diameter (1/4", 6.35 datasheet)</t>
+  </si>
+  <si>
+    <t>Enclosure Cutout: 7 mm diameter (1/4", 6.35 datasheet)</t>
+  </si>
+  <si>
+    <t>Enclosure cutout: 11.05 mm diameter datasheet (11 actual)</t>
+  </si>
+  <si>
+    <t>Enclosure cutout: 7.93 mm diameter datasheet (8 mm actual)</t>
   </si>
 </sst>
 </file>
@@ -1302,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6075A09A-FCAE-4580-9D34-D8EB72A353D0}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1397,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="6" t="str">
-        <f t="shared" ref="E2:E44" si="0">B2&amp;" "&amp;C2&amp;" "&amp;D2</f>
+        <f t="shared" ref="E2:E45" si="0">B2&amp;" "&amp;C2&amp;" "&amp;D2</f>
         <v>CAP CER 1uF 10V 10% 0603 SMD</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1398,13 +1419,13 @@
     </row>
     <row r="3" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
@@ -1421,13 +1442,13 @@
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="19" t="s">
         <v>245</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1981,7 +2002,7 @@
         <v>RES 1K 1% 1/10W 0603 SMD</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G20" s="4">
         <v>3</v>
@@ -2548,7 +2569,7 @@
         <v>7</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="J37" s="15" t="s">
         <v>212</v>
@@ -2586,6 +2607,9 @@
       <c r="H38" s="15" t="s">
         <v>7</v>
       </c>
+      <c r="I38" s="15" t="s">
+        <v>252</v>
+      </c>
       <c r="J38" s="15" t="s">
         <v>138</v>
       </c>
@@ -2601,13 +2625,13 @@
         <v>1053091204</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C39" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>221</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>222</v>
       </c>
       <c r="E39" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2620,13 +2644,13 @@
         <v>7</v>
       </c>
       <c r="J39" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="13" t="s">
         <v>224</v>
-      </c>
-      <c r="K39" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2634,7 +2658,7 @@
         <v>1053071204</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E40" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2647,13 +2671,13 @@
         <v>7</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K40" s="15" t="s">
         <v>19</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2661,7 +2685,7 @@
         <v>1053002200</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E41" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2674,24 +2698,24 @@
         <v>7</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K41" s="15" t="s">
         <v>19</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="C42" s="15" t="s">
         <v>231</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>232</v>
       </c>
       <c r="E42" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2703,6 +2727,9 @@
       <c r="H42" s="15" t="s">
         <v>7</v>
       </c>
+      <c r="I42" s="15" t="s">
+        <v>253</v>
+      </c>
       <c r="J42" s="15" t="s">
         <v>55</v>
       </c>
@@ -2710,18 +2737,18 @@
         <v>19</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B43" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>236</v>
       </c>
       <c r="E43" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2740,25 +2767,25 @@
         <v>19</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="C44" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>240</v>
-      </c>
       <c r="E44" s="15" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">PRESS-FIT NUT 2-56 0.07" HEIGHT </v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G44" s="4">
         <v>2</v>
@@ -2767,15 +2794,41 @@
         <v>7</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="G45" s="4"/>
+      <c r="A45" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E45" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">LIGHTPIPE THREADED  </v>
+      </c>
+      <c r="G45" s="4">
+        <v>1</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="46" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>

</xml_diff>

<commit_message>
Added diode to second battery pack
</commit_message>
<xml_diff>
--- a/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
+++ b/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prl242\repositories\Iridium_9603_Beacon\Eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93B384A-365D-4006-B323-CC24BED97B06}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A01AC76-3538-4CE9-8F47-8B14BD8C62FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{3D564F82-D3D8-4CC0-A9F4-2EE497ABD49A}"/>
   </bookViews>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6075A09A-FCAE-4580-9D34-D8EB72A353D0}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,7 +2455,7 @@
         <v>192</v>
       </c>
       <c r="G34" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H34" s="15" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Board as submitted to AAPCB
</commit_message>
<xml_diff>
--- a/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
+++ b/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prl242\repositories\Iridium_9603_Beacon\Eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A01AC76-3538-4CE9-8F47-8B14BD8C62FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B07F7E-011F-459C-8CA8-06EE5A055E2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{3D564F82-D3D8-4CC0-A9F4-2EE497ABD49A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D564F82-D3D8-4CC0-A9F4-2EE497ABD49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="280">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -333,24 +333,12 @@
     <t>732-1783-1-ND</t>
   </si>
   <si>
-    <t>COM-11821</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED DISCRETE </t>
-  </si>
-  <si>
-    <t>SERIAL RGB</t>
-  </si>
-  <si>
     <t>LED1</t>
   </si>
   <si>
     <t>Sparkfun</t>
   </si>
   <si>
-    <t>1568-1800-ND</t>
-  </si>
-  <si>
     <t>150080RS75000</t>
   </si>
   <si>
@@ -426,9 +414,6 @@
     <t>C9,C13</t>
   </si>
   <si>
-    <t>D1,D2,D3,D4</t>
-  </si>
-  <si>
     <t>Q1,Q2,Q3,Q4</t>
   </si>
   <si>
@@ -874,6 +859,96 @@
   </si>
   <si>
     <t>Enclosure cutout: 7.93 mm diameter datasheet (8 mm actual)</t>
+  </si>
+  <si>
+    <t>D1,D2,D3,D4,D6</t>
+  </si>
+  <si>
+    <t>COM-13667</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>SMD LED - RGB WS2812B</t>
+  </si>
+  <si>
+    <t>Must be this part number.</t>
+  </si>
+  <si>
+    <t>94669A100</t>
+  </si>
+  <si>
+    <t>ALUMINUM SPACER</t>
+  </si>
+  <si>
+    <t>M2.5 Screw Size, 4.5 mm OD, 6 mm Long</t>
+  </si>
+  <si>
+    <t>92185A081</t>
+  </si>
+  <si>
+    <t>316 STAINLESS SOCKET HEAD SCREW</t>
+  </si>
+  <si>
+    <t>2-56 7/16" Long</t>
+  </si>
+  <si>
+    <t>90107A003</t>
+  </si>
+  <si>
+    <t>316 STAINLESS WASHER</t>
+  </si>
+  <si>
+    <t>#2 Screw, 0.094" ID, 0.25" OD</t>
+  </si>
+  <si>
+    <t>92147A410</t>
+  </si>
+  <si>
+    <t>316 STAINLESS SPLIT WASHER</t>
+  </si>
+  <si>
+    <t>#2 Screw, 0.094" ID, 0.172" OD</t>
+  </si>
+  <si>
+    <t>92290A113</t>
+  </si>
+  <si>
+    <t>M3 x 0.5 Thread, 8 mm Long</t>
+  </si>
+  <si>
+    <t>90965A130</t>
+  </si>
+  <si>
+    <t>M3 Screw, 3.2 mm ID, 7 mm OD</t>
+  </si>
+  <si>
+    <t>92153A416</t>
+  </si>
+  <si>
+    <t>M3 Screw, 3.4 mm ID, 6.2 mm OD</t>
+  </si>
+  <si>
+    <t>94500A226</t>
+  </si>
+  <si>
+    <t>316 STAINLESS BUTTON HEAD HEX SCREW</t>
+  </si>
+  <si>
+    <t>M4 x 0.7 mm, 8 mm Long</t>
+  </si>
+  <si>
+    <t>90965A150</t>
+  </si>
+  <si>
+    <t>M4 Screw, 4.3 mm ID, 0.9 mm OD</t>
+  </si>
+  <si>
+    <t>92153A418</t>
+  </si>
+  <si>
+    <t>M4 Screw, 4.4 mm ID, 7.6 mm OD</t>
   </si>
 </sst>
 </file>
@@ -990,9 +1065,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1007,6 +1079,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1321,10 +1394,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6075A09A-FCAE-4580-9D34-D8EB72A353D0}">
-  <dimension ref="A1:N49"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1460,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1397,11 +1473,11 @@
         <v>17</v>
       </c>
       <c r="E2" s="6" t="str">
-        <f t="shared" ref="E2:E45" si="0">B2&amp;" "&amp;C2&amp;" "&amp;D2</f>
+        <f t="shared" ref="E2:E56" si="0">B2&amp;" "&amp;C2&amp;" "&amp;D2</f>
         <v>CAP CER 1uF 10V 10% 0603 SMD</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G2" s="4">
         <v>4</v>
@@ -1418,14 +1494,14 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
-        <v>246</v>
+      <c r="A3" s="18" t="s">
+        <v>241</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
@@ -1435,24 +1511,24 @@
         <v>CAP CER 12 pF 50V 5% 0603 SMD</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G3" s="4">
         <v>2</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="19" t="s">
-        <v>245</v>
+      <c r="L3" s="18" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1469,7 +1545,7 @@
         <v>CAP CER 10uF 10V 10% 0805 SMD</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G4" s="4">
         <v>6</v>
@@ -1481,12 +1557,12 @@
       <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1503,7 +1579,7 @@
         <v>CAP CER 0.1UF 25V 10% 0805 SMD</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G5" s="4">
         <v>2</v>
@@ -1515,12 +1591,12 @@
       <c r="K5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1551,12 +1627,12 @@
       <c r="K6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1584,12 +1660,12 @@
       <c r="K7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1617,12 +1693,12 @@
       <c r="K8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1650,12 +1726,12 @@
       <c r="K9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1683,12 +1759,12 @@
       <c r="K10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1698,17 +1774,17 @@
         <v>59</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>DIODE SCHOTTKY 20V 1A SOD-123 SMD</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>105</v>
+        <v>250</v>
       </c>
       <c r="G11" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>60</v>
@@ -1716,12 +1792,12 @@
       <c r="K11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1749,12 +1825,12 @@
       <c r="K12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1782,1069 +1858,1406 @@
       <c r="K13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>74</v>
+      <c r="A14" s="11" t="s">
+        <v>251</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>76</v>
+        <v>252</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>LED DISCRETE  SERIAL RGB SMD</v>
+        <v>LED RGB SMD</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
+      <c r="I14" s="8" t="s">
+        <v>254</v>
+      </c>
       <c r="J14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="13" t="s">
+      <c r="D15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>LED RED CLEAR 0805 SMD</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LED RED CLEAR 0805 SMD</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="13" t="s">
+      <c r="K15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>88</v>
-      </c>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>MOSFET P-CHAN 24V SOT-23 SMD</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>106</v>
+      <c r="F16" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="G16" s="4">
         <v>4</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="K16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="13" t="s">
+      <c r="D17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>TRANS NPN 40V 0.6A SOT-23 SMD</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>TRANS NPN 40V 0.6A SOT-23 SMD</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="K17" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 100K 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>107</v>
+      <c r="F18" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="G18" s="4">
         <v>6</v>
       </c>
-      <c r="J18" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="15" t="s">
+      <c r="J18" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 12K 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>112</v>
+      <c r="F19" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="G19" s="4">
         <v>1</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="K19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="15" t="s">
+    </row>
+    <row r="20" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 1K 1% 1/10W 0603 SMD</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>242</v>
+      <c r="F20" s="14" t="s">
+        <v>237</v>
       </c>
       <c r="G20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="15" t="s">
+      <c r="K20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 47K 1% 1/10W 0603 SMD</v>
       </c>
-      <c r="F21" s="15" t="s">
-        <v>119</v>
+      <c r="F21" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="G21" s="4">
         <v>1</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="15" t="s">
+      <c r="K21" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 10 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>123</v>
+      <c r="F22" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="G22" s="4">
         <v>1</v>
       </c>
-      <c r="J22" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" s="15" t="s">
+      <c r="J22" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 30K 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>128</v>
+      <c r="F23" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="G23" s="4">
         <v>1</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="K23" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D24" s="15" t="s">
+    </row>
+    <row r="24" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 10K 1% 1/8W 0603 SMD</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>132</v>
+      <c r="F24" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="G24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="K24" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D25" s="15" t="s">
+      <c r="J24" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SWITCH TACTILE SPST-NO 0.05A 32V SMD</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>137</v>
+      <c r="F25" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="G25" s="4">
         <v>1</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="K25" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="13" t="s">
+      <c r="E26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>IC VOLT DET 2.32V LOW SOT-23-3 SMD</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>IC VOLT DET 2.32V LOW SOT-23-3 SMD</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>144</v>
       </c>
       <c r="G26" s="4">
         <v>1</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="13" t="s">
+      <c r="E27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>IC REG LINEAR 3.3V 500mA SOT-23-5 SMD</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E27" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>IC REG LINEAR 3.3V 500mA SOT-23-5 SMD</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>151</v>
       </c>
       <c r="G27" s="4">
         <v>1</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="J27" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="K27" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27" s="13" t="s">
+      <c r="E28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>IC SUPERCAP CHARGER 150mA 10-DFN SMD</v>
+      </c>
+      <c r="F28" s="14" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E28" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>IC SUPERCAP CHARGER 150mA 10-DFN SMD</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="G28" s="4">
         <v>1</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="J28" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>IC ALTIMETER I2C  8-LGA SMD</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>159</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>IC ALTIMETER I2C  8-LGA SMD</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>164</v>
       </c>
       <c r="G29" s="4">
         <v>1</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>IC MCU 32BIT 256KB FLASH  48-QFN</v>
+      </c>
+      <c r="F30" s="14" t="s">
         <v>165</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="E30" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>IC MCU 32BIT 256KB FLASH  48-QFN</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>170</v>
       </c>
       <c r="G30" s="4">
         <v>1</v>
       </c>
-      <c r="J30" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" s="15" t="str">
+      <c r="J30" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" s="14" t="str">
         <f t="shared" si="0"/>
         <v>IC RECEIVER GPS/GNSS  18LCC SMD</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>175</v>
+      <c r="F31" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="G31" s="4">
         <v>1</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="K31" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" s="13" t="s">
+      <c r="E32" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>IC VREF SHUNT 1.25V 8-MSOP SMD</v>
+      </c>
+      <c r="F32" s="14" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="E32" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>IC VREF SHUNT 1.25V 8-MSOP SMD</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>182</v>
       </c>
       <c r="G32" s="4">
         <v>1</v>
       </c>
-      <c r="J32" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K32" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" s="15" t="s">
+      <c r="J32" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="15" t="str">
+      <c r="E33" s="14" t="str">
         <f t="shared" si="0"/>
         <v>CRYSTAL 32.7680 kHz 12.5 pF SMD</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>187</v>
+      <c r="F33" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="G33" s="4">
         <v>1</v>
       </c>
-      <c r="J33" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" s="13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="16">
+      <c r="J33" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="15">
         <v>92</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="E34" s="15" t="str">
+      <c r="B34" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E34" s="14" t="str">
         <f t="shared" si="0"/>
         <v>BATT CONTACT CLIP  PC PIN</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>192</v>
+      <c r="F34" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="G34" s="4">
         <v>12</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="J34" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="K34" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L34" s="13" t="s">
+      <c r="E35" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CAP 1F -10% +30% 2.7V RADIAL</v>
+      </c>
+      <c r="F35" s="14" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="E35" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>CAP 1F -10% +30% 2.7V RADIAL</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>199</v>
       </c>
       <c r="G35" s="4">
         <v>2</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="J35" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>RELAY TELECOM DPDT 2A 250V PC PIN</v>
+      </c>
+      <c r="F36" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L35" s="13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="E36" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>RELAY TELECOM DPDT 2A 250V PC PIN</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>205</v>
       </c>
       <c r="G36" s="4">
         <v>1</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="H36" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="J36" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CONN SMA JACK STR 50 OHM BOARD EDGE</v>
+      </c>
+      <c r="F37" s="14" t="s">
         <v>206</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="E37" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>CONN SMA JACK STR 50 OHM BOARD EDGE</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>211</v>
       </c>
       <c r="G37" s="4">
         <v>2</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="H37" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="B38" s="15" t="s">
+      <c r="I37" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="E38" s="15" t="str">
+    </row>
+    <row r="38" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E38" s="14" t="str">
         <f t="shared" si="0"/>
         <v>SWITCH TOGGLE SPDT 5A 120V PC PIN</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>216</v>
+      <c r="F38" s="14" t="s">
+        <v>211</v>
       </c>
       <c r="G38" s="4">
         <v>1</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="H38" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I38" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="K38" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L38" s="13" t="s">
+      <c r="I38" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="15">
+        <v>1053091204</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="16">
-        <v>1053091204</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="E39" s="15" t="str">
+      <c r="C39" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E39" s="14" t="str">
         <f t="shared" si="0"/>
         <v>CONN HEADER VERT MALE 4POS 2.5MM PIN</v>
       </c>
       <c r="G39" s="4">
         <v>2</v>
       </c>
-      <c r="H39" s="15" t="s">
+      <c r="H39" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J39" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="K39" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="16">
+      <c r="J39" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="15">
         <v>1053071204</v>
       </c>
-      <c r="B40" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="E40" s="15" t="str">
+      <c r="B40" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E40" s="14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">NANOFIT RCPT  </v>
       </c>
       <c r="G40" s="4">
         <v>2</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J40" s="15" t="s">
+      <c r="J40" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="15">
+        <v>1053002200</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NANOFIT CRIMP TERM  </v>
+      </c>
+      <c r="G41" s="4">
+        <v>10</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="K40" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L40" s="13" t="s">
+    </row>
+    <row r="42" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C42" s="14" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="16">
-        <v>1053002200</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="E41" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">NANOFIT CRIMP TERM  </v>
-      </c>
-      <c r="G41" s="4">
-        <v>25</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="K41" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L41" s="13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="E42" s="15" t="str">
+      <c r="E42" s="14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">CONN RCPT FMALE 4POS </v>
       </c>
       <c r="G42" s="4">
         <v>2</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H42" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="J42" s="15" t="s">
+      <c r="I42" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="J42" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="K42" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E43" s="15" t="str">
+      <c r="K42" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" s="14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">CBL ASSY U.FL PLUG-PLUG 1.969" </v>
       </c>
       <c r="G43" s="4">
         <v>1</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H43" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J43" s="15" t="s">
+      <c r="J43" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="K43" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L43" s="13" t="s">
+      <c r="K43" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E44" s="14" t="str">
+        <f>B44&amp;" "&amp;C44&amp;" "&amp;D44</f>
+        <v xml:space="preserve">LIGHTPIPE THREADED  </v>
+      </c>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="K44" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PRESS-FIT NUT 2-56 0.07" HEIGHT </v>
+      </c>
+      <c r="F45" s="14" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="E44" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PRESS-FIT NUT 2-56 0.07" HEIGHT </v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="G44" s="4">
+      <c r="G45" s="4">
         <v>2</v>
       </c>
-      <c r="H44" s="15" t="s">
+      <c r="H45" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K44" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="E45" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">LIGHTPIPE THREADED  </v>
-      </c>
-      <c r="G45" s="4">
-        <v>1</v>
-      </c>
-      <c r="H45" s="15" t="s">
+      <c r="K45" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="E46" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ALUMINUM SPACER M2.5 Screw Size, 4.5 mm OD, 6 mm Long </v>
+      </c>
+      <c r="G46" s="4">
+        <v>2</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="K45" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="G46" s="4"/>
-    </row>
-    <row r="47" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-    </row>
-    <row r="48" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-    </row>
-    <row r="49" spans="1:1" s="10" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="9"/>
+      <c r="K46" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L46" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="E47" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS SOCKET HEAD SCREW 2-56 7/16" Long </v>
+      </c>
+      <c r="G47" s="4">
+        <v>2</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="E48" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS WASHER #2 Screw, 0.094" ID, 0.25" OD </v>
+      </c>
+      <c r="G48" s="4">
+        <v>2</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E49" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS SPLIT WASHER #2 Screw, 0.094" ID, 0.172" OD </v>
+      </c>
+      <c r="G49" s="4">
+        <v>2</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K49" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L49" s="14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="9" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS SOCKET HEAD SCREW M3 x 0.5 Thread, 8 mm Long </v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="4">
+        <v>7</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L50" s="14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS WASHER M3 Screw, 3.2 mm ID, 7 mm OD </v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="4">
+        <v>7</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L51" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="M51" s="9"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS SPLIT WASHER M3 Screw, 3.4 mm ID, 6.2 mm OD </v>
+      </c>
+      <c r="F52" s="14"/>
+      <c r="G52" s="4">
+        <v>7</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L52" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="M52" s="9"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS BUTTON HEAD HEX SCREW M4 x 0.7 mm, 8 mm Long </v>
+      </c>
+      <c r="F53" s="14"/>
+      <c r="G53" s="4">
+        <v>6</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L53" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="M53" s="9"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS WASHER M4 Screw, 4.3 mm ID, 0.9 mm OD </v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="4">
+        <v>6</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L54" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="M54" s="9"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">316 STAINLESS SPLIT WASHER M4 Screw, 4.4 mm ID, 7.6 mm OD </v>
+      </c>
+      <c r="F55" s="14"/>
+      <c r="G55" s="4">
+        <v>6</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="L55" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="M55" s="9"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+      <c r="F56" s="14"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="9"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="9"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="45" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated BOM. started new operational code. Iridium9603NBeacon_V5M_XDATA
</commit_message>
<xml_diff>
--- a/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
+++ b/Eagle/Iridium Board V5M - BOM for AAPCB - Revision 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prl242\repositories\Iridium_9603_Beacon\Eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B07F7E-011F-459C-8CA8-06EE5A055E2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E012CF-8A70-4609-9B2A-14614EECFA1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D564F82-D3D8-4CC0-A9F4-2EE497ABD49A}"/>
   </bookViews>
@@ -861,9 +861,6 @@
     <t>Enclosure cutout: 7.93 mm diameter datasheet (8 mm actual)</t>
   </si>
   <si>
-    <t>D1,D2,D3,D4,D6</t>
-  </si>
-  <si>
     <t>COM-13667</t>
   </si>
   <si>
@@ -949,6 +946,9 @@
   </si>
   <si>
     <t>M4 Screw, 4.4 mm ID, 7.6 mm OD</t>
+  </si>
+  <si>
+    <t>D1,D2,D3,D4,D5</t>
   </si>
 </sst>
 </file>
@@ -1038,48 +1038,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,8 +1396,8 @@
   </sheetPr>
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1491,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>241</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1523,7 +1520,7 @@
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="16" t="s">
         <v>240</v>
       </c>
     </row>
@@ -1759,12 +1756,12 @@
       <c r="K10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="L10" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1781,7 +1778,7 @@
         <v>DIODE SCHOTTKY 20V 1A SOD-123 SMD</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="G11" s="4">
         <v>5</v>
@@ -1792,12 +1789,12 @@
       <c r="K11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1825,12 +1822,12 @@
       <c r="K12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1858,19 +1855,19 @@
       <c r="K13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>53</v>
@@ -1886,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>75</v>
@@ -1895,1365 +1892,1365 @@
         <v>75</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>LED RED CLEAR 0805 SMD</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="8" t="s">
         <v>79</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="12" t="s">
+      <c r="K15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>MOSFET P-CHAN 24V SOT-23 SMD</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="4">
         <v>4</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="12" t="s">
+      <c r="K16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>TRANS NPN 40V 0.6A SOT-23 SMD</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="8" t="s">
         <v>91</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="K17" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="12" t="s">
+      <c r="K17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 100K 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="8" t="s">
         <v>102</v>
       </c>
       <c r="G18" s="4">
         <v>6</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="K18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="12" t="s">
+      <c r="K18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 12K 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="8" t="s">
         <v>107</v>
       </c>
       <c r="G19" s="4">
         <v>1</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="K19" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="12" t="s">
+      <c r="K19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 1K 1% 1/10W 0603 SMD</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="8" t="s">
         <v>237</v>
       </c>
       <c r="G20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="12" t="s">
+      <c r="K20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 47K 1% 1/10W 0603 SMD</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="8" t="s">
         <v>114</v>
       </c>
       <c r="G21" s="4">
         <v>1</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="12" t="s">
+      <c r="K21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 10 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="8" t="s">
         <v>118</v>
       </c>
       <c r="G22" s="4">
         <v>1</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="K22" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="12" t="s">
+      <c r="K22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 30K 1% 1/8W 0805 SMD</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="8" t="s">
         <v>123</v>
       </c>
       <c r="G23" s="4">
         <v>1</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="K23" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="12" t="s">
+      <c r="K23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RES 10K 1% 1/8W 0603 SMD</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="8" t="s">
         <v>127</v>
       </c>
       <c r="G24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="K24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L24" s="12" t="s">
+      <c r="K24" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="8" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SWITCH TACTILE SPST-NO 0.05A 32V SMD</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="8" t="s">
         <v>132</v>
       </c>
       <c r="G25" s="4">
         <v>1</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="K25" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="12" t="s">
+      <c r="K25" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="8" t="s">
         <v>138</v>
       </c>
       <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>IC VOLT DET 2.32V LOW SOT-23-3 SMD</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="8" t="s">
         <v>139</v>
       </c>
       <c r="G26" s="4">
         <v>1</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K26" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="12" t="s">
+      <c r="K26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+    <row r="27" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="8" t="s">
         <v>145</v>
       </c>
       <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>IC REG LINEAR 3.3V 500mA SOT-23-5 SMD</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="8" t="s">
         <v>146</v>
       </c>
       <c r="G27" s="4">
         <v>1</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="K27" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27" s="12" t="s">
+      <c r="K27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="8" t="s">
         <v>152</v>
       </c>
       <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>IC SUPERCAP CHARGER 150mA 10-DFN SMD</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="8" t="s">
         <v>153</v>
       </c>
       <c r="G28" s="4">
         <v>1</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="J28" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="K28" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="12" t="s">
+      <c r="K28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="11" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+    <row r="29" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="8" t="s">
         <v>158</v>
       </c>
       <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>IC ALTIMETER I2C  8-LGA SMD</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="8" t="s">
         <v>159</v>
       </c>
       <c r="G29" s="4">
         <v>1</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="J29" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="K29" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29" s="12" t="s">
+      <c r="K29" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="8" t="s">
         <v>164</v>
       </c>
       <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>IC MCU 32BIT 256KB FLASH  48-QFN</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="8" t="s">
         <v>165</v>
       </c>
       <c r="G30" s="4">
         <v>1</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K30" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" s="12" t="s">
+      <c r="K30" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
+    <row r="31" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E31" s="14" t="str">
+      <c r="E31" s="8" t="str">
         <f t="shared" si="0"/>
         <v>IC RECEIVER GPS/GNSS  18LCC SMD</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="8" t="s">
         <v>170</v>
       </c>
       <c r="G31" s="4">
         <v>1</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K31" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" s="12" t="s">
+      <c r="K31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
+    <row r="32" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="14" t="str">
+      <c r="E32" s="8" t="str">
         <f t="shared" si="0"/>
         <v>IC VREF SHUNT 1.25V 8-MSOP SMD</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="8" t="s">
         <v>177</v>
       </c>
       <c r="G32" s="4">
         <v>1</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="K32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="12" t="s">
+      <c r="K32" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+    <row r="33" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="14" t="str">
+      <c r="E33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>CRYSTAL 32.7680 kHz 12.5 pF SMD</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="8" t="s">
         <v>182</v>
       </c>
       <c r="G33" s="4">
         <v>1</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="K33" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" s="12" t="s">
+      <c r="K33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="15">
+    <row r="34" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="13">
         <v>92</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E34" s="14" t="str">
+      <c r="E34" s="8" t="str">
         <f t="shared" si="0"/>
         <v>BATT CONTACT CLIP  PC PIN</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="8" t="s">
         <v>187</v>
       </c>
       <c r="G34" s="4">
         <v>12</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="K34" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L34" s="12" t="s">
+      <c r="K34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
+    <row r="35" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E35" s="14" t="str">
+      <c r="E35" s="8" t="str">
         <f t="shared" si="0"/>
         <v>CAP 1F -10% +30% 2.7V RADIAL</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="8" t="s">
         <v>194</v>
       </c>
       <c r="G35" s="4">
         <v>2</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="K35" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L35" s="12" t="s">
+      <c r="K35" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+    <row r="36" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E36" s="14" t="str">
+      <c r="E36" s="8" t="str">
         <f t="shared" si="0"/>
         <v>RELAY TELECOM DPDT 2A 250V PC PIN</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="8" t="s">
         <v>200</v>
       </c>
       <c r="G36" s="4">
         <v>1</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J36" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="K36" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" s="12" t="s">
+      <c r="K36" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
+    <row r="37" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E37" s="14" t="str">
+      <c r="E37" s="8" t="str">
         <f t="shared" si="0"/>
         <v>CONN SMA JACK STR 50 OHM BOARD EDGE</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="8" t="s">
         <v>206</v>
       </c>
       <c r="G37" s="4">
         <v>2</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="J37" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K37" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L37" s="12" t="s">
+      <c r="K37" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37" s="11" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+    <row r="38" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E38" s="14" t="str">
+      <c r="E38" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SWITCH TOGGLE SPDT 5A 120V PC PIN</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="8" t="s">
         <v>211</v>
       </c>
       <c r="G38" s="4">
         <v>1</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="H38" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="K38" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L38" s="12" t="s">
+      <c r="K38" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38" s="11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="15">
+    <row r="39" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
         <v>1053091204</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E39" s="14" t="str">
+      <c r="E39" s="8" t="str">
         <f t="shared" si="0"/>
         <v>CONN HEADER VERT MALE 4POS 2.5MM PIN</v>
       </c>
       <c r="G39" s="4">
         <v>2</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="H39" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J39" s="14" t="s">
+      <c r="J39" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="K39" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L39" s="12" t="s">
+      <c r="K39" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="11" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="15">
+    <row r="40" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="13">
         <v>1053071204</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E40" s="14" t="str">
+      <c r="E40" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">NANOFIT RCPT  </v>
       </c>
       <c r="G40" s="4">
         <v>2</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="H40" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="K40" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L40" s="12" t="s">
+      <c r="K40" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="15">
+    <row r="41" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="13">
         <v>1053002200</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E41" s="14" t="str">
+      <c r="E41" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">NANOFIT CRIMP TERM  </v>
       </c>
       <c r="G41" s="4">
         <v>10</v>
       </c>
-      <c r="H41" s="14" t="s">
+      <c r="H41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J41" s="14" t="s">
+      <c r="J41" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="K41" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L41" s="12" t="s">
+      <c r="K41" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="11" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
+    <row r="42" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="E42" s="14" t="str">
+      <c r="E42" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">CONN RCPT FMALE 4POS </v>
       </c>
       <c r="G42" s="4">
         <v>2</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="14" t="s">
+      <c r="I42" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="J42" s="14" t="s">
+      <c r="J42" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="K42" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" s="12" t="s">
+      <c r="K42" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="11" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
+    <row r="43" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="E43" s="14" t="str">
+      <c r="E43" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">CBL ASSY U.FL PLUG-PLUG 1.969" </v>
       </c>
       <c r="G43" s="4">
         <v>1</v>
       </c>
-      <c r="H43" s="14" t="s">
+      <c r="H43" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J43" s="14" t="s">
+      <c r="J43" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="K43" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L43" s="12" t="s">
+      <c r="K43" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" s="11" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
+    <row r="44" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="E44" s="14" t="str">
+      <c r="E44" s="8" t="str">
         <f>B44&amp;" "&amp;C44&amp;" "&amp;D44</f>
         <v xml:space="preserve">LIGHTPIPE THREADED  </v>
       </c>
       <c r="G44" s="4">
         <v>1</v>
       </c>
-      <c r="H44" s="14" t="s">
+      <c r="H44" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I44" s="14" t="s">
+      <c r="I44" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="K44" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L44" s="12" t="s">
+      <c r="K44" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+    <row r="45" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="E45" s="14" t="str">
+      <c r="E45" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">PRESS-FIT NUT 2-56 0.07" HEIGHT </v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="8" t="s">
         <v>236</v>
       </c>
       <c r="G45" s="4">
         <v>2</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="H45" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K45" s="14" t="s">
+      <c r="K45" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L45" s="16" t="s">
+      <c r="L45" s="14" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="C46" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="E46" s="14" t="str">
+      <c r="E46" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ALUMINUM SPACER M2.5 Screw Size, 4.5 mm OD, 6 mm Long </v>
       </c>
       <c r="G46" s="4">
         <v>2</v>
       </c>
-      <c r="H46" s="14" t="s">
+      <c r="H46" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K46" s="14" t="s">
+      <c r="K46" s="8" t="s">
         <v>235</v>
       </c>
       <c r="L46" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="C47" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C47" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="E47" s="14" t="str">
+      <c r="E47" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS SOCKET HEAD SCREW 2-56 7/16" Long </v>
       </c>
       <c r="G47" s="4">
         <v>2</v>
       </c>
-      <c r="H47" s="14" t="s">
+      <c r="H47" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K47" s="14" t="s">
+      <c r="K47" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L47" s="13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
+      <c r="L47" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="C48" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="E48" s="14" t="str">
+      <c r="E48" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS WASHER #2 Screw, 0.094" ID, 0.25" OD </v>
       </c>
       <c r="G48" s="4">
         <v>2</v>
       </c>
-      <c r="H48" s="14" t="s">
+      <c r="H48" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K48" s="14" t="s">
+      <c r="K48" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L48" s="13" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
+      <c r="L48" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="C49" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="E49" s="14" t="str">
+      <c r="E49" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS SPLIT WASHER #2 Screw, 0.094" ID, 0.172" OD </v>
       </c>
       <c r="G49" s="4">
         <v>2</v>
       </c>
-      <c r="H49" s="14" t="s">
+      <c r="H49" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K49" s="14" t="s">
+      <c r="K49" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L49" s="14" t="s">
-        <v>264</v>
+      <c r="L49" s="8" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:13" s="9" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="B50" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14" t="str">
+      <c r="D50" s="8"/>
+      <c r="E50" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS SOCKET HEAD SCREW M3 x 0.5 Thread, 8 mm Long </v>
       </c>
-      <c r="F50" s="14"/>
+      <c r="F50" s="8"/>
       <c r="G50" s="4">
         <v>7</v>
       </c>
-      <c r="H50" s="14" t="s">
+      <c r="H50" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14" t="s">
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L50" s="14" t="s">
-        <v>267</v>
+      <c r="L50" s="8" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="B51" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14" t="str">
+      <c r="D51" s="8"/>
+      <c r="E51" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS WASHER M3 Screw, 3.2 mm ID, 7 mm OD </v>
       </c>
-      <c r="F51" s="14"/>
+      <c r="F51" s="8"/>
       <c r="G51" s="4">
         <v>7</v>
       </c>
-      <c r="H51" s="14" t="s">
+      <c r="H51" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14" t="s">
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L51" s="14" t="s">
-        <v>269</v>
+      <c r="L51" s="8" t="s">
+        <v>268</v>
       </c>
       <c r="M51" s="9"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="B52" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14" t="str">
+      <c r="D52" s="8"/>
+      <c r="E52" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS SPLIT WASHER M3 Screw, 3.4 mm ID, 6.2 mm OD </v>
       </c>
-      <c r="F52" s="14"/>
+      <c r="F52" s="8"/>
       <c r="G52" s="4">
         <v>7</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14" t="s">
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L52" s="14" t="s">
-        <v>271</v>
+      <c r="L52" s="8" t="s">
+        <v>270</v>
       </c>
       <c r="M52" s="9"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="C53" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="C53" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14" t="str">
+      <c r="D53" s="8"/>
+      <c r="E53" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS BUTTON HEAD HEX SCREW M4 x 0.7 mm, 8 mm Long </v>
       </c>
-      <c r="F53" s="14"/>
+      <c r="F53" s="8"/>
       <c r="G53" s="4">
         <v>6</v>
       </c>
-      <c r="H53" s="14" t="s">
+      <c r="H53" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14" t="s">
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L53" s="14" t="s">
-        <v>273</v>
+      <c r="L53" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="M53" s="9"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="B54" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14" t="str">
+      <c r="D54" s="8"/>
+      <c r="E54" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS WASHER M4 Screw, 4.3 mm ID, 0.9 mm OD </v>
       </c>
-      <c r="F54" s="14"/>
+      <c r="F54" s="8"/>
       <c r="G54" s="4">
         <v>6</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="H54" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14" t="s">
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L54" s="14" t="s">
-        <v>276</v>
+      <c r="L54" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="M54" s="9"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B55" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14" t="str">
+      <c r="D55" s="8"/>
+      <c r="E55" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">316 STAINLESS SPLIT WASHER M4 Screw, 4.4 mm ID, 7.6 mm OD </v>
       </c>
-      <c r="F55" s="14"/>
+      <c r="F55" s="8"/>
       <c r="G55" s="4">
         <v>6</v>
       </c>
-      <c r="H55" s="14" t="s">
+      <c r="H55" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14" t="s">
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="L55" s="14" t="s">
-        <v>278</v>
+      <c r="L55" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="M55" s="9"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14" t="str">
+      <c r="A56" s="12"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="F56" s="14"/>
+      <c r="F56" s="8"/>
       <c r="G56" s="4"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
       <c r="M56" s="9"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
       <c r="G57" s="4"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
       <c r="M57" s="9"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
       <c r="M58" s="9"/>
     </row>
   </sheetData>

</xml_diff>